<commit_message>
retouches to the GeneSet pipeline, not very important
</commit_message>
<xml_diff>
--- a/resources/genes_of_interest.xlsx
+++ b/resources/genes_of_interest.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JQ/Documents/_CODE REPOS/GitHub/Da_RNAseq/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F9D6AAAF-CFF3-4E46-AE82-A3C857816BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8216D0BC-F13F-A344-9D40-E774C7BE44A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="36040" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="genes_of_interest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="150">
   <si>
     <t>ac</t>
   </si>
@@ -317,13 +330,166 @@
   </si>
   <si>
     <t>gene_symbol</t>
+  </si>
+  <si>
+    <t>Patr-1</t>
+  </si>
+  <si>
+    <t>translation</t>
+  </si>
+  <si>
+    <t>P-bodies</t>
+  </si>
+  <si>
+    <t>Ref func</t>
+  </si>
+  <si>
+    <t>Ref expn</t>
+  </si>
+  <si>
+    <t>10.1016/j.celrep.2022.111495</t>
+  </si>
+  <si>
+    <t>Hey</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>10.7554/eLife.44745</t>
+  </si>
+  <si>
+    <t>zfh2</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pgen.1008553</t>
+  </si>
+  <si>
+    <t>ZFH</t>
+  </si>
+  <si>
+    <t>AdoR</t>
+  </si>
+  <si>
+    <t>Adgf-A</t>
+  </si>
+  <si>
+    <t>10.1073/pnas.1900103117</t>
+  </si>
+  <si>
+    <t>proliferation</t>
+  </si>
+  <si>
+    <t>Dutta</t>
+  </si>
+  <si>
+    <t>RnrL</t>
+  </si>
+  <si>
+    <t>dNTP synth</t>
+  </si>
+  <si>
+    <t>dATP signaling</t>
+  </si>
+  <si>
+    <t>receptor</t>
+  </si>
+  <si>
+    <t>deaminase</t>
+  </si>
+  <si>
+    <t>EB</t>
+  </si>
+  <si>
+    <t>10.1016/j.isci.2020.100954</t>
+  </si>
+  <si>
+    <t>RnrS</t>
+  </si>
+  <si>
+    <t>10.1016/j.isci.2020.100954, Dutta</t>
+  </si>
+  <si>
+    <t>Eip75B</t>
+  </si>
+  <si>
+    <t>10.7554/eLife.55795</t>
+  </si>
+  <si>
+    <t>Nuclear receptor</t>
+  </si>
+  <si>
+    <t>E(y)2</t>
+  </si>
+  <si>
+    <t>Sgf11</t>
+  </si>
+  <si>
+    <t>Cp190</t>
+  </si>
+  <si>
+    <t>Nup98</t>
+  </si>
+  <si>
+    <t>chromatin</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>10.7554/eLife.62312</t>
+  </si>
+  <si>
+    <t>mod(mdg4)</t>
+  </si>
+  <si>
+    <t>Not</t>
+  </si>
+  <si>
+    <t>Zfh2</t>
+  </si>
+  <si>
+    <t>cyc</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>apt</t>
+  </si>
+  <si>
+    <t>CG11247</t>
+  </si>
+  <si>
+    <t>jumu</t>
+  </si>
+  <si>
+    <t>CG30403</t>
+  </si>
+  <si>
+    <t>Sox100B</t>
+  </si>
+  <si>
+    <t>10.1073/pnas.1719169115</t>
+  </si>
+  <si>
+    <t>10.1073/pnas.1719169115, Dutta</t>
+  </si>
+  <si>
+    <t>TNF</t>
+  </si>
+  <si>
+    <t>Ilp6</t>
+  </si>
+  <si>
+    <t>10.1016/j.stemcr.2020.01.003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -458,8 +624,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,6 +825,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -806,9 +1016,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1163,12 +1385,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,9 +1398,11 @@
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="11" max="11" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -1206,8 +1430,14 @@
       <c r="I1" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1466,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1265,7 +1495,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1294,7 +1524,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1323,7 +1553,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1352,7 +1582,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1611,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1410,7 +1640,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1439,7 +1669,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1465,7 +1695,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1494,7 +1724,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1523,7 +1753,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1552,7 +1782,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1581,7 +1811,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1607,7 +1837,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2848,7 +3078,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -2874,7 +3104,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -2897,7 +3127,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -2920,7 +3150,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2943,7 +3173,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -2969,7 +3199,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -2995,7 +3225,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -3021,7 +3251,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -3047,7 +3277,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -3073,7 +3303,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -3099,7 +3329,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -3125,7 +3355,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -3151,7 +3381,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -3177,7 +3407,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -3201,6 +3431,551 @@
       </c>
       <c r="I78" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H79" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I79" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J79" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K79" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I80" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J80" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K80" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I83" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J83" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K83" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J106" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>